<commit_message>
Progress on reading excel files. Seems to work in general but there is an issue with POST requests.
</commit_message>
<xml_diff>
--- a/godocExample.xlsx
+++ b/godocExample.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="GET Tests" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="GET_Tests" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="POST Tests" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -205,17 +205,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.7142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.9642857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.969387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.31632653061225"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="4.47959183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.4642857142857"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.1836734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.43367346938776"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="2.53571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="2.42857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -316,17 +316,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9642857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.4387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.969387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.57142857142857"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="4.47959183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.4642857142857"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.1836734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.43367346938776"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="2.53571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="2.42857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Making testing work by adding an Euqals function to HTTPTest.
There is still a long way to go with this and I'm not sure if I like the implementation yet.
</commit_message>
<xml_diff>
--- a/godocExample.xlsx
+++ b/godocExample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="GET_Tests" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
     <t xml:space="preserve">Godoc GET basic HTTP</t>
   </si>
   <si>
-    <t xml:space="preserve">http://localhost:8080</t>
+    <t xml:space="preserve">http://localhost:6060</t>
   </si>
   <si>
     <t xml:space="preserve">GET</t>
@@ -87,11 +87,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -114,6 +115,87 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
@@ -121,15 +203,57 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -137,8 +261,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -162,17 +301,73 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -181,14 +376,90 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="22">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -199,28 +470,30 @@
   </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="J1:K1 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.4030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.99489795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="2.29591836734694"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="2.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="0" t="s">
@@ -229,7 +502,7 @@
       <c r="F1" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="I1" s="2"/>
+      <c r="I1" s="3"/>
       <c r="J1" s="0" t="n">
         <v>2</v>
       </c>
@@ -241,7 +514,7 @@
       <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -253,7 +526,7 @@
       <c r="F2" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="I2" s="3"/>
       <c r="J2" s="0" t="n">
         <v>2</v>
       </c>
@@ -265,7 +538,7 @@
       <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="0" t="s">
@@ -280,7 +553,7 @@
       <c r="H3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="I3" s="3" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -292,11 +565,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" display="http://localhost:8080"/>
-    <hyperlink ref="B2" r:id="rId2" display="http://localhost:8080"/>
-    <hyperlink ref="B3" r:id="rId3" display="http://localhost:8080"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -314,28 +582,30 @@
   </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1:K1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.4030612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="2.29591836734694"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="2.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="0" t="s">
@@ -347,7 +617,7 @@
       <c r="F1" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="I1" s="2"/>
+      <c r="I1" s="3"/>
       <c r="J1" s="0" t="n">
         <v>2</v>
       </c>
@@ -359,10 +629,10 @@
       <c r="A2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -374,7 +644,7 @@
       <c r="F2" s="0" t="n">
         <v>200</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="I2" s="3"/>
       <c r="J2" s="0" t="n">
         <v>2</v>
       </c>
@@ -386,10 +656,10 @@
       <c r="A3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="0" t="s">
@@ -407,7 +677,7 @@
       <c r="H3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="I3" s="3" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Improved excel import testing.
</commit_message>
<xml_diff>
--- a/godocExample.xlsx
+++ b/godocExample.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t xml:space="preserve">Godoc GET basic HTTP</t>
   </si>
@@ -470,22 +470,22 @@
   </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="2.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="2.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
   <sheetData>
@@ -540,6 +540,9 @@
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>2</v>
@@ -582,7 +585,7 @@
   </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
@@ -590,14 +593,14 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="2.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="2.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.67"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Added a tester set timeout.
</commit_message>
<xml_diff>
--- a/godocExample.xlsx
+++ b/godocExample.xlsx
@@ -468,18 +468,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.84"/>
@@ -509,6 +509,9 @@
       <c r="K1" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="L1" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -533,6 +536,9 @@
       <c r="K2" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="L2" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -564,6 +570,9 @@
         <v>2</v>
       </c>
       <c r="K3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L3" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -583,10 +592,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -627,8 +636,11 @@
       <c r="K1" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="L1" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="113.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="186.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>12</v>
       </c>
@@ -654,8 +666,11 @@
       <c r="K2" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="L2" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="113.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="186.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>14</v>
       </c>
@@ -688,6 +703,9 @@
         <v>2</v>
       </c>
       <c r="K3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L3" s="0" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cleaned the README and set more sensible unit for timeouts.
</commit_message>
<xml_diff>
--- a/godocExample.xlsx
+++ b/godocExample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GET_Tests" sheetId="1" state="visible" r:id="rId2"/>
@@ -470,8 +470,8 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1:L3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -510,7 +510,7 @@
         <v>2</v>
       </c>
       <c r="L1" s="0" t="n">
-        <v>2</v>
+        <v>750</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -537,7 +537,7 @@
         <v>2</v>
       </c>
       <c r="L2" s="0" t="n">
-        <v>2</v>
+        <v>750</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -573,7 +573,7 @@
         <v>2</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>2</v>
+        <v>750</v>
       </c>
     </row>
   </sheetData>
@@ -594,8 +594,8 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1:L3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -637,10 +637,10 @@
         <v>2</v>
       </c>
       <c r="L1" s="0" t="n">
-        <v>2</v>
+        <v>750</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="186.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="22.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>12</v>
       </c>
@@ -667,10 +667,10 @@
         <v>2</v>
       </c>
       <c r="L2" s="0" t="n">
-        <v>2</v>
+        <v>750</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="186.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="24.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>14</v>
       </c>
@@ -706,7 +706,7 @@
         <v>2</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>2</v>
+        <v>750</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed an issue where defaults are set incorrectly for timeout, time elapse, and retries.
</commit_message>
<xml_diff>
--- a/godocExample.xlsx
+++ b/godocExample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="GET_Tests" sheetId="1" state="visible" r:id="rId2"/>
@@ -470,7 +470,7 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
@@ -572,9 +572,6 @@
       <c r="K3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="L3" s="0" t="n">
-        <v>750</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -594,8 +591,8 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -636,9 +633,6 @@
       <c r="K1" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="L1" s="0" t="n">
-        <v>750</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="22.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">

</xml_diff>

<commit_message>
Substituting in the regular logger.
</commit_message>
<xml_diff>
--- a/godocExample.xlsx
+++ b/godocExample.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="GET_Tests" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="GET Tests" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="POST Tests" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Auth Tests" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -470,7 +471,7 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
@@ -712,4 +713,30 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>